<commit_message>
Add graph for monthly date
</commit_message>
<xml_diff>
--- a/Data/Datos.xlsx
+++ b/Data/Datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\Documents\Felipe\Programacion\PrecioInmueblesMercadoLibre\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ABF9E21-30C5-4B0A-8ADC-FB55AA42D1D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E3E976-1999-4EC2-BF7F-4FD1332DDCAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>fecha</t>
   </si>
@@ -238,6 +238,12 @@
   </si>
   <si>
     <t>4/5/2024</t>
+  </si>
+  <si>
+    <t>preciocasamensual</t>
+  </si>
+  <si>
+    <t>precioapartamentomensual</t>
   </si>
 </sst>
 </file>
@@ -595,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="M60" sqref="M60"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -604,6 +610,8 @@
     <col min="1" max="1" width="8.44140625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -616,6 +624,12 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -970,7 +984,7 @@
         <v>234130</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>22</v>
       </c>
@@ -981,7 +995,7 @@
         <v>225645</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>23</v>
       </c>
@@ -992,7 +1006,7 @@
         <v>212784</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>24</v>
       </c>
@@ -1003,7 +1017,7 @@
         <v>210472</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>25</v>
       </c>
@@ -1014,7 +1028,7 @@
         <v>217211</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>51</v>
       </c>
@@ -1024,8 +1038,14 @@
       <c r="C37" s="2">
         <v>212331</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D37" s="2">
+        <v>298935</v>
+      </c>
+      <c r="E37" s="2">
+        <v>231285</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>52</v>
       </c>
@@ -1036,7 +1056,7 @@
         <v>211506</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>53</v>
       </c>
@@ -1047,7 +1067,7 @@
         <v>212188</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>54</v>
       </c>
@@ -1058,7 +1078,7 @@
         <v>213869</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>55</v>
       </c>
@@ -1069,7 +1089,7 @@
         <v>215005</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>56</v>
       </c>
@@ -1080,7 +1100,7 @@
         <v>216909</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>57</v>
       </c>
@@ -1091,7 +1111,7 @@
         <v>210766</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>58</v>
       </c>
@@ -1102,7 +1122,7 @@
         <v>221497</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>59</v>
       </c>
@@ -1113,7 +1133,7 @@
         <v>208198</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>60</v>
       </c>
@@ -1124,7 +1144,7 @@
         <v>215042</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>61</v>
       </c>
@@ -1135,7 +1155,7 @@
         <v>213350</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>62</v>
       </c>
@@ -1324,7 +1344,7 @@
         <v>194264</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>67</v>
       </c>
@@ -1335,7 +1355,7 @@
         <v>196871</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>66</v>
       </c>
@@ -1345,8 +1365,14 @@
       <c r="C66" s="2">
         <v>197622</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D66" s="2">
+        <v>287383</v>
+      </c>
+      <c r="E66" s="2">
+        <v>208325</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>68</v>
       </c>
@@ -1357,7 +1383,7 @@
         <v>200534</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
         <v>69</v>
       </c>
@@ -1368,7 +1394,7 @@
         <v>205744</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
         <v>70</v>
       </c>

</xml_diff>

<commit_message>
Clean Code of graph generator
</commit_message>
<xml_diff>
--- a/Data/Datos.xlsx
+++ b/Data/Datos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felip\Documents\Felipe\Programacion\PrecioInmueblesMercadoLibre\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E3E976-1999-4EC2-BF7F-4FD1332DDCAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761ACB30-86E6-45D4-9178-E99ACC9EA20F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>fecha</t>
   </si>
@@ -244,6 +244,27 @@
   </si>
   <si>
     <t>precioapartamentomensual</t>
+  </si>
+  <si>
+    <t>5/52024</t>
+  </si>
+  <si>
+    <t>6/5/2024</t>
+  </si>
+  <si>
+    <t>7/5/2024</t>
+  </si>
+  <si>
+    <t>8/5/2024</t>
+  </si>
+  <si>
+    <t>9/5/2024</t>
+  </si>
+  <si>
+    <t>26/4/2024</t>
+  </si>
+  <si>
+    <t>10/5/2024</t>
   </si>
 </sst>
 </file>
@@ -599,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:J76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G62" sqref="G62"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1312,97 +1333,176 @@
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="2" t="s">
-        <v>63</v>
+      <c r="A62" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="B62" s="2">
-        <v>297589</v>
+        <v>296955</v>
       </c>
       <c r="C62" s="2">
-        <v>201335</v>
+        <v>203915</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B63" s="2">
-        <v>294812</v>
+        <v>297589</v>
       </c>
       <c r="C63" s="2">
-        <v>195805</v>
+        <v>201335</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B64" s="2">
+        <v>294812</v>
+      </c>
+      <c r="C64" s="2">
+        <v>195805</v>
+      </c>
+      <c r="G64" s="7"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B64" s="2">
+      <c r="B65" s="2">
         <v>290873</v>
       </c>
-      <c r="C64" s="2">
+      <c r="C65" s="2">
         <v>194264</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" s="2" t="s">
+      <c r="G65" s="7"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B65" s="2">
+      <c r="B66" s="2">
         <v>285952</v>
       </c>
-      <c r="C65" s="2">
+      <c r="C66" s="2">
         <v>196871</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="2" t="s">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B66" s="2">
+      <c r="B67" s="2">
         <v>282768</v>
       </c>
-      <c r="C66" s="2">
+      <c r="C67" s="2">
         <v>197622</v>
       </c>
-      <c r="D66" s="2">
+      <c r="D67" s="2">
         <v>287383</v>
       </c>
-      <c r="E66" s="2">
+      <c r="E67" s="2">
         <v>208325</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" s="2" t="s">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B67" s="2">
+      <c r="B68" s="2">
         <v>277379</v>
       </c>
-      <c r="C67" s="2">
+      <c r="C68" s="2">
         <v>200534</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" s="5" t="s">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A69" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B68" s="2">
+      <c r="B69" s="2">
         <v>273819</v>
       </c>
-      <c r="C68" s="2">
+      <c r="C69" s="2">
         <v>205744</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69" s="5" t="s">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A70" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B69" s="2">
+      <c r="B70" s="2">
         <v>273371</v>
       </c>
-      <c r="C69" s="2">
+      <c r="C70" s="2">
         <v>210773</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A71" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B71" s="2">
+        <v>271891</v>
+      </c>
+      <c r="C71" s="2">
+        <v>215745</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B72" s="2">
+        <v>276455</v>
+      </c>
+      <c r="C72" s="2">
+        <v>215925</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A73" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B73" s="2">
+        <v>269692</v>
+      </c>
+      <c r="C73" s="2">
+        <v>213855</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A74" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B74" s="2">
+        <v>275778</v>
+      </c>
+      <c r="C74" s="2">
+        <v>209558</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A75" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B75" s="2">
+        <v>285859</v>
+      </c>
+      <c r="C75" s="2">
+        <v>209261</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A76" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B76" s="2">
+        <v>297189</v>
+      </c>
+      <c r="C76" s="2">
+        <v>210616</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edit in month graph
</commit_message>
<xml_diff>
--- a/Data/Datos.xlsx
+++ b/Data/Datos.xlsx
@@ -435,10 +435,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J87"/>
+  <dimension ref="A1:J97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -476,6 +476,11 @@
           <t>precioapartamentomensual</t>
         </is>
       </c>
+      <c r="F1" s="7" t="inlineStr">
+        <is>
+          <t>mes</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="5" t="inlineStr">
@@ -962,6 +967,11 @@
       <c r="E37" s="4" t="n">
         <v>231285</v>
       </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Marzo</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="5" t="inlineStr">
@@ -1362,6 +1372,11 @@
       <c r="E67" s="4" t="n">
         <v>208325</v>
       </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Abril</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="9" t="inlineStr">
@@ -1627,6 +1642,136 @@
       </c>
       <c r="C87" t="n">
         <v>209922</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>22/5/2024</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>273736</v>
+      </c>
+      <c r="C88" t="n">
+        <v>203236</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>23/5/2024</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>272089</v>
+      </c>
+      <c r="C89" t="n">
+        <v>204473</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>24/5/2024</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>290788</v>
+      </c>
+      <c r="C90" t="n">
+        <v>208759</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>25/5/2024</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>274724</v>
+      </c>
+      <c r="C91" t="n">
+        <v>204444</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>26/5/2024</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>271899</v>
+      </c>
+      <c r="C92" t="n">
+        <v>203806</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>27/5/2024</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>274246</v>
+      </c>
+      <c r="C93" t="n">
+        <v>204864</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>28/5/2024</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>280584</v>
+      </c>
+      <c r="C94" t="n">
+        <v>203810</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>29/5/2024</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>282538</v>
+      </c>
+      <c r="C95" t="n">
+        <v>205653</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>30/5/2024</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>284018</v>
+      </c>
+      <c r="C96" t="n">
+        <v>210566</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>31/5/2024</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>278300</v>
+      </c>
+      <c r="C97" t="n">
+        <v>210430</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add response in update data
</commit_message>
<xml_diff>
--- a/Data/Datos.xlsx
+++ b/Data/Datos.xlsx
@@ -435,10 +435,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J97"/>
+  <dimension ref="A1:J113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="F99" sqref="F99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -1774,6 +1774,225 @@
         <v>210430</v>
       </c>
     </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>1/6/2024</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>277503</v>
+      </c>
+      <c r="C98" t="n">
+        <v>208978</v>
+      </c>
+      <c r="D98" t="n">
+        <v>278968</v>
+      </c>
+      <c r="E98" t="n">
+        <v>208193</v>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>Mayo</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2/6/2024</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>277211</v>
+      </c>
+      <c r="C99" t="n">
+        <v>208949</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>3/6/2024</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>274283</v>
+      </c>
+      <c r="C100" t="n">
+        <v>211621</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>4/6/2024</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>273135</v>
+      </c>
+      <c r="C101" t="n">
+        <v>209914</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>5/6/2024</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>272523</v>
+      </c>
+      <c r="C102" t="n">
+        <v>204424</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>6/6/2024</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>267370</v>
+      </c>
+      <c r="C103" t="n">
+        <v>204806</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>7/6/2024</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>274828</v>
+      </c>
+      <c r="C104" t="n">
+        <v>207520</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>8/6/2024</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>266926</v>
+      </c>
+      <c r="C105" t="n">
+        <v>208226</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>9/6/2024</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>271366</v>
+      </c>
+      <c r="C106" t="n">
+        <v>207723</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>10/6/2024</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>270523</v>
+      </c>
+      <c r="C107" t="n">
+        <v>209239</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>11/6/2024</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>271634</v>
+      </c>
+      <c r="C108" t="n">
+        <v>215625</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>12/6/2024</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>268474</v>
+      </c>
+      <c r="C109" t="n">
+        <v>214037</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>13/6/2024</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>267590</v>
+      </c>
+      <c r="C110" t="n">
+        <v>212338</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>14/6/2024</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>267179</v>
+      </c>
+      <c r="C111" t="n">
+        <v>211049</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>15/6/2024</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>267017</v>
+      </c>
+      <c r="C112" t="n">
+        <v>209942</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>16/6/2024</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>266778</v>
+      </c>
+      <c r="C113" t="n">
+        <v>210528</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>